<commit_message>
Moved settings files to new settings folder
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pauls Playwright Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pauls PW Project\Pauls-Test-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B595B8C-F992-481A-9EF1-17BDDE1F8073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E078C988-2172-44CC-BC71-0545E303D550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0CDD907C-F4A0-4B21-ABA0-3910FEB2D339}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>To Do List</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>Importing csv data into framework</t>
+  </si>
+  <si>
+    <t>Implement appsettings</t>
+  </si>
+  <si>
+    <t>implement scenariokeys across steps</t>
   </si>
 </sst>
 </file>
@@ -452,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{975AACD9-D029-4677-A326-E99884AFBA83}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,26 +496,39 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added import test and methods
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pauls PW Project\Pauls-Test-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E078C988-2172-44CC-BC71-0545E303D550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F929E3-6616-45CD-91C8-7420B87D3C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0CDD907C-F4A0-4B21-ABA0-3910FEB2D339}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>To Do List</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>implement scenariokeys across steps</t>
+  </si>
+  <si>
+    <t>Implement CI/CD</t>
   </si>
 </sst>
 </file>
@@ -458,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{975AACD9-D029-4677-A326-E99884AFBA83}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,6 +509,9 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -530,6 +536,11 @@
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>